<commit_message>
EC4: Graphs LUT/Register x ap_fixed reformatted.
The graphs which relate how LUTs and registers increase with fixed-point precision were reformatted in response to comments during the revision of the EC4 manuscript.
</commit_message>
<xml_diff>
--- a/EC4-FPGA_Braking/explainable_braking_SW/2023 05 12 Revision 6/ap_fixed and LUTs-Reg analysis/LUTs and Registers Analysis.xlsx
+++ b/EC4-FPGA_Braking/explainable_braking_SW/2023 05 12 Revision 6/ap_fixed and LUTs-Reg analysis/LUTs and Registers Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Arnaldo\Documents\Documentos Toti\Escola Politécnica - USP\Pós-Graduação\Doutorado\14 - Relatórios Técnicos\07 - Estudo de Caso 4\2023 09 21 Revisão 17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Arnaldo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -123,7 +123,7 @@
           <c:x val="0.18280475366509155"/>
           <c:y val="6.5131433173605854E-2"/>
           <c:w val="0.78097600611449225"/>
-          <c:h val="0.64592251772127274"/>
+          <c:h val="0.57656464237111515"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -401,11 +401,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116320936"/>
-        <c:axId val="116315056"/>
+        <c:axId val="145515824"/>
+        <c:axId val="145515432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116320936"/>
+        <c:axId val="145515824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -434,7 +434,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr algn="ctr" rtl="0">
-                  <a:defRPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="fr-FR" sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -447,7 +447,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -458,10 +458,38 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:rPr>
-                  <a:t>ap_fixed&lt;</a:t>
+                  <a:t>Bit Width of Fixed-Point Precision </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>(n) </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>with 12 Decimal Bits (ap_fixed&lt;</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="1" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -475,7 +503,7 @@
                   <a:t>n</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -486,8 +514,19 @@
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:rPr>
-                  <a:t>, 12&gt;</a:t>
+                  <a:t>,12&gt;)</a:t>
                 </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -495,8 +534,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.38529026985796982"/>
-              <c:y val="0.80745304994711076"/>
+              <c:x val="0.1911914392960867"/>
+              <c:y val="0.74788299387622104"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -512,7 +551,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
-                <a:defRPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="fr-FR" sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
@@ -550,7 +589,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -565,13 +604,13 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116315056"/>
+        <c:crossAx val="145515432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116315056"/>
+        <c:axId val="145515432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
@@ -599,7 +638,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr lang="fr-FR" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -612,7 +651,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:rPr lang="fr-FR" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
@@ -642,7 +681,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr lang="fr-FR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr lang="fr-FR" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
@@ -680,7 +719,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -695,9 +734,10 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116320936"/>
+        <c:crossAx val="145515824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -721,10 +761,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16056437523818115"/>
-          <c:y val="0.91716520828897174"/>
+          <c:x val="0.20007617188816576"/>
+          <c:y val="0.91716521293465048"/>
           <c:w val="0.67413899086290696"/>
-          <c:h val="4.9889472821674136E-2"/>
+          <c:h val="7.4359018822409639E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -740,7 +780,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -824,7 +864,7 @@
           <c:x val="0.18712885154061626"/>
           <c:y val="6.0237491064702151E-2"/>
           <c:w val="0.77663813673617599"/>
-          <c:h val="0.63375625470849239"/>
+          <c:h val="0.57724023078805808"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1102,11 +1142,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="116315840"/>
-        <c:axId val="116317016"/>
+        <c:axId val="145494656"/>
+        <c:axId val="145495048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116315840"/>
+        <c:axId val="145494656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -1135,7 +1175,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1148,23 +1188,38 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400">
-                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="0" baseline="0">
+                    <a:effectLst/>
                   </a:rPr>
-                  <a:t>ap_fixed&lt;</a:t>
+                  <a:t>Bit Width of Fixed-Point Precision </a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400" i="1">
-                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="1" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>(n) </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>with 12 Decimal Bits (ap_fixed&lt;</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="1" baseline="0">
+                    <a:effectLst/>
                   </a:rPr>
                   <a:t>n</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400">
-                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                  <a:rPr lang="fr-FR" sz="1300" b="1" i="0" baseline="0">
+                    <a:effectLst/>
                   </a:rPr>
-                  <a:t>, 12&gt;</a:t>
+                  <a:t>,12&gt;)</a:t>
                 </a:r>
+                <a:endParaRPr lang="pt-BR" sz="1300">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1172,8 +1227,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.41419329987673881"/>
-              <c:y val="0.7863223951800451"/>
+              <c:x val="0.20134194418508145"/>
+              <c:y val="0.73633987666428757"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1189,7 +1244,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1300" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1227,7 +1282,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1242,13 +1297,13 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116317016"/>
+        <c:crossAx val="145495048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116317016"/>
+        <c:axId val="145495048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2000"/>
@@ -1276,7 +1331,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1289,7 +1344,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400">
+                  <a:rPr lang="en-US" sz="1400" b="1">
                     <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                   </a:rPr>
                   <a:t>Registers</a:t>
@@ -1301,8 +1356,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.6115953512942424E-3"/>
-              <c:y val="0.25436437518424537"/>
+              <c:x val="2.6115260919182489E-3"/>
+              <c:y val="0.20219560160819089"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1318,7 +1373,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1356,7 +1411,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1371,7 +1426,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="116315840"/>
+        <c:crossAx val="145494656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1416,7 +1471,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1300" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2594,8 +2649,8 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>29882</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -2608,7 +2663,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DC66FF20-8493-4949-6F07-AD9437F33824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC66FF20-8493-4949-6F07-AD9437F33824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2630,8 +2685,8 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>436554</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>26893</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
@@ -2644,7 +2699,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B15B8588-AB7D-5F3C-9007-F18175FF8C11}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B15B8588-AB7D-5F3C-9007-F18175FF8C11}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2964,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>